<commit_message>
Creer un systeme d'enreigistrement, recupere les donnes et le sstoque dans une feuille excel grace a la bibliotheque org.apache.poi
</commit_message>
<xml_diff>
--- a/SystenEnregistre/Donnees.xlsx
+++ b/SystenEnregistre/Donnees.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="39">
   <si>
     <t xml:space="preserve">Ad      </t>
   </si>
@@ -113,6 +113,25 @@
   </si>
   <si>
     <t xml:space="preserve">Tongolo vers makepe adıyaman / kahta
+</t>
+  </si>
+  <si>
+    <t>Barthez</t>
+  </si>
+  <si>
+    <t>Tonlio</t>
+  </si>
+  <si>
+    <t>0 201 - 789 - 52 - 30</t>
+  </si>
+  <si>
+    <t>izmir</t>
+  </si>
+  <si>
+    <t>buca</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Horozluhan Mh izmir / buca
 </t>
   </si>
 </sst>
@@ -158,7 +177,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:I7"/>
+  <dimension ref="A1:I8"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -376,6 +395,35 @@
         <v>17</v>
       </c>
     </row>
+    <row r="8">
+      <c r="A8" t="s" s="0">
+        <v>33</v>
+      </c>
+      <c r="B8" t="s" s="0">
+        <v>34</v>
+      </c>
+      <c r="C8" t="s" s="0">
+        <v>35</v>
+      </c>
+      <c r="D8" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="E8" t="s" s="0">
+        <v>22</v>
+      </c>
+      <c r="F8" t="s" s="0">
+        <v>36</v>
+      </c>
+      <c r="G8" t="s" s="0">
+        <v>37</v>
+      </c>
+      <c r="H8" t="s" s="0">
+        <v>38</v>
+      </c>
+      <c r="I8" t="s" s="0">
+        <v>26</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>